<commit_message>
hari om sheet updated
</commit_message>
<xml_diff>
--- a/Accounts.xlsx
+++ b/Accounts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14235" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -554,7 +554,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -589,7 +589,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1128,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,13 +1353,13 @@
         <v>35</v>
       </c>
       <c r="G8" s="29">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H8" s="29" t="s">
         <v>14</v>
       </c>
       <c r="I8" s="29">
-        <v>700</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="I9" s="29">
         <f>SUM(I5:I8)</f>
-        <v>5505</v>
+        <v>6065</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1404,7 +1404,7 @@
       <c r="H11" s="29"/>
       <c r="I11" s="29">
         <f>SUM(I9:I10)</f>
-        <v>5403</v>
+        <v>5963</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1433,7 +1433,7 @@
       <c r="H13" s="29"/>
       <c r="I13" s="29">
         <f>SUM(I11:I12)</f>
-        <v>8403</v>
+        <v>8963</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1476,7 +1476,7 @@
       <c r="H15" s="14"/>
       <c r="I15" s="14">
         <f>SUM(I13:I14)</f>
-        <v>9243</v>
+        <v>9803</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1504,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
hari om on dated 28 aug
</commit_message>
<xml_diff>
--- a/Accounts.xlsx
+++ b/Accounts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14235" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>Missing</t>
+  </si>
+  <si>
+    <t>Hari om 28.8.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hari om </t>
+  </si>
+  <si>
+    <t>Farma (9x15)</t>
+  </si>
+  <si>
+    <t>3set</t>
   </si>
 </sst>
 </file>
@@ -494,24 +506,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -520,6 +514,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -870,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,17 +1029,17 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="38"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="42"/>
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1112,14 +1124,26 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="15">
+        <v>43705</v>
+      </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="C10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="14">
+        <v>35</v>
+      </c>
       <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="H10" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1679,25 +1703,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="6"/>
-    <col min="2" max="2" width="6.42578125" style="43" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="37" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="43" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="37" customWidth="1"/>
     <col min="5" max="7" width="11.42578125" style="6"/>
     <col min="8" max="8" width="23.7109375" style="6" customWidth="1"/>
-    <col min="9" max="10" width="11.42578125" style="6"/>
-    <col min="11" max="11" width="11.42578125" style="43"/>
+    <col min="9" max="9" width="11.42578125" style="6"/>
+    <col min="10" max="10" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="37"/>
     <col min="12" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -1718,18 +1743,18 @@
       <c r="G1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="44">
+      <c r="K1" s="38">
         <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
+      <c r="A2" s="44"/>
       <c r="B2" s="7" t="s">
         <v>18</v>
       </c>
@@ -1748,12 +1773,12 @@
       <c r="G2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="41"/>
-      <c r="J2" s="42" t="s">
+      <c r="H2" s="45"/>
+      <c r="J2" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="44">
-        <v>39</v>
+      <c r="K2" s="38">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1775,107 +1800,129 @@
       <c r="H3" s="9">
         <v>77100</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="38">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="38"/>
+      <c r="J4" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="44">
+      <c r="K4" s="38">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="44"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="44"/>
-    </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="J5" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="38">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="44">
+      <c r="B6" s="38">
         <v>1</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="38">
         <v>9654753654</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="J6" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="38">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="44">
+      <c r="B7" s="38">
         <v>2</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="44">
+      <c r="D7" s="38">
         <v>9999006467</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="38"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="44">
+      <c r="B8" s="38">
         <v>3</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="44">
+      <c r="D8" s="38">
         <v>9560521439</v>
       </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="38"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="44">
+      <c r="B9" s="38">
         <v>4</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="44">
+      <c r="D9" s="38">
         <v>8766304037</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="38"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="44">
+      <c r="B10" s="38">
         <v>5</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="38">
         <v>9654416298</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>